<commit_message>
Fixed Screen copy, added Actions
</commit_message>
<xml_diff>
--- a/Docs/Rogue Packets.xlsx
+++ b/Docs/Rogue Packets.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lbloomqu\Desktop\MultiRogueLike\MultiRogueLike\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="165" windowWidth="27795" windowHeight="14055"/>
   </bookViews>
@@ -15,12 +10,12 @@
     <sheet name="C64 to Server" sheetId="5" r:id="rId1"/>
     <sheet name="Server to C64" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="81">
   <si>
     <t>Byte#</t>
   </si>
@@ -118,9 +113,6 @@
     <t>Actions</t>
   </si>
   <si>
-    <t>No action</t>
-  </si>
-  <si>
     <t>Move</t>
   </si>
   <si>
@@ -256,10 +248,16 @@
     <t>0=Current Cell</t>
   </si>
   <si>
-    <t>2=Left Hand</t>
-  </si>
-  <si>
-    <t>3=Right Hand</t>
+    <t>1=Left Hand</t>
+  </si>
+  <si>
+    <t>2=Right Hand</t>
+  </si>
+  <si>
+    <t>Keys</t>
+  </si>
+  <si>
+    <t>No action (heartbeat)</t>
   </si>
 </sst>
 </file>
@@ -484,7 +482,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -519,7 +517,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -728,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M89"/>
+  <dimension ref="B1:P89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -745,7 +743,7 @@
     <col min="7" max="7" width="3.140625" style="15" customWidth="1"/>
     <col min="8" max="8" width="3.42578125" style="15" customWidth="1"/>
     <col min="9" max="9" width="2.85546875" style="15" customWidth="1"/>
-    <col min="10" max="10" width="16" style="15" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" style="15" customWidth="1"/>
     <col min="11" max="11" width="24" style="15" customWidth="1"/>
     <col min="12" max="12" width="16.85546875" style="15" customWidth="1"/>
     <col min="13" max="13" width="15.140625" style="15" customWidth="1"/>
@@ -1130,7 +1128,7 @@
     <col min="16134" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C1" s="16" t="s">
         <v>3</v>
       </c>
@@ -1138,7 +1136,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
@@ -1152,10 +1150,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="19"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="15">
         <v>0</v>
       </c>
@@ -1169,7 +1167,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="15">
         <v>1</v>
       </c>
@@ -1177,7 +1175,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="15">
         <v>2</v>
       </c>
@@ -1185,7 +1183,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="15">
         <v>3</v>
       </c>
@@ -1193,49 +1191,52 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="15">
         <v>4</v>
       </c>
       <c r="C9" s="22"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="15">
         <v>5</v>
       </c>
       <c r="C10" s="22"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="15">
         <v>6</v>
       </c>
       <c r="C11" s="22"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" s="15">
         <v>7</v>
       </c>
       <c r="C12" s="22"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="P12" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="15">
         <v>8</v>
       </c>
       <c r="C13" s="22"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="15">
         <v>9</v>
       </c>
       <c r="C14" s="22"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="15">
         <v>10</v>
       </c>
       <c r="C15" s="22"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="15">
         <v>11</v>
       </c>
@@ -1268,13 +1269,13 @@
         <v>31</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
@@ -1286,13 +1287,13 @@
         <v>0</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="L21" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M21" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
@@ -1307,16 +1308,16 @@
         <v>1</v>
       </c>
       <c r="J22" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K22" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M22" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.2">
@@ -1331,16 +1332,16 @@
         <v>2</v>
       </c>
       <c r="J23" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M23" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
@@ -1354,13 +1355,13 @@
         <v>3</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K24" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L24" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
@@ -1371,10 +1372,10 @@
         <v>8</v>
       </c>
       <c r="D25" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="24" t="s">
         <v>49</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>50</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="24"/>
@@ -1383,13 +1384,13 @@
         <v>4</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K25" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L25" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
@@ -1397,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>12</v>
@@ -1410,13 +1411,13 @@
         <v>5</v>
       </c>
       <c r="J26" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="K26" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="K26" s="15" t="s">
-        <v>44</v>
-      </c>
       <c r="L26" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
@@ -1424,10 +1425,10 @@
         <v>2</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
@@ -1436,13 +1437,13 @@
         <v>6</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K27" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L27" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
@@ -1450,10 +1451,10 @@
         <v>3</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
@@ -1462,13 +1463,13 @@
         <v>7</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K28" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L28" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
@@ -1476,7 +1477,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F29" s="24"/>
       <c r="G29" s="24"/>
@@ -1485,13 +1486,13 @@
         <v>8</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K29" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L29" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.2">
@@ -1505,13 +1506,13 @@
         <v>9</v>
       </c>
       <c r="J30" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K30" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L30" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
@@ -1519,10 +1520,10 @@
         <v>0</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
@@ -1532,11 +1533,11 @@
         <v>10</v>
       </c>
       <c r="J31" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K31" s="24"/>
       <c r="L31" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.2">
@@ -1544,7 +1545,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D32" s="24"/>
       <c r="F32" s="24"/>
@@ -1552,7 +1553,7 @@
       <c r="H32" s="24"/>
       <c r="K32" s="24"/>
       <c r="L32" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
@@ -1560,7 +1561,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
@@ -1592,7 +1593,7 @@
         <v>50</v>
       </c>
       <c r="J35" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K35" s="24"/>
     </row>
@@ -1607,7 +1608,7 @@
         <v>51</v>
       </c>
       <c r="J36" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K36" s="24"/>
     </row>
@@ -1880,7 +1881,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="8.25" x14ac:dyDescent="0.15"/>
@@ -2375,7 +2376,7 @@
         <v>20</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.15">
@@ -2384,7 +2385,7 @@
         <v>21</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.15">
@@ -2402,7 +2403,7 @@
         <v>17</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Switched to keystroke input
</commit_message>
<xml_diff>
--- a/Docs/Rogue Packets.xlsx
+++ b/Docs/Rogue Packets.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="225" windowWidth="27795" windowHeight="13995" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="225" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="C64 to Server" sheetId="5" r:id="rId1"/>
     <sheet name="Server to C64" sheetId="6" r:id="rId2"/>
+    <sheet name="Actions" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="81">
   <si>
     <t>Byte#</t>
   </si>
@@ -50,9 +51,6 @@
     <t>Direction</t>
   </si>
   <si>
-    <t>See =&gt;</t>
-  </si>
-  <si>
     <t>Packet Type = 129</t>
   </si>
   <si>
@@ -113,9 +111,6 @@
     <t>Move</t>
   </si>
   <si>
-    <t>Action</t>
-  </si>
-  <si>
     <t>Cast Spell</t>
   </si>
   <si>
@@ -125,9 +120,6 @@
     <t>For duplicate actions</t>
   </si>
   <si>
-    <t>Parameter to above actions, if needed</t>
-  </si>
-  <si>
     <t>Use Item</t>
   </si>
   <si>
@@ -164,12 +156,6 @@
     <t>Sent by C64 when player does sometihing</t>
   </si>
   <si>
-    <t>Parameter 1</t>
-  </si>
-  <si>
-    <t>Parameter 2 (if needed)</t>
-  </si>
-  <si>
     <t>Pause Game</t>
   </si>
   <si>
@@ -251,9 +237,6 @@
     <t>2=Right Hand</t>
   </si>
   <si>
-    <t>Keys</t>
-  </si>
-  <si>
     <t>No action (heartbeat)</t>
   </si>
   <si>
@@ -267,6 +250,15 @@
   </si>
   <si>
     <t>Into Left or Right Hand</t>
+  </si>
+  <si>
+    <t>Keystroke</t>
+  </si>
+  <si>
+    <t>Keystrokes faked by joystick routine if needed</t>
+  </si>
+  <si>
+    <t>reserved</t>
   </si>
 </sst>
 </file>
@@ -391,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -425,7 +417,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,17 +726,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P89"/>
+  <dimension ref="B1:J89"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="15" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="26" style="15" customWidth="1"/>
+    <col min="3" max="3" width="31" style="15" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="15" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="15" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="15"/>
@@ -1137,15 +1128,15 @@
     <col min="16134" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C1" s="16" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" s="18" customFormat="1" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
@@ -1159,10 +1150,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:16" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="19"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="15">
         <v>0</v>
       </c>
@@ -1173,139 +1164,112 @@
         <v>8</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="15">
         <v>1</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="15">
         <v>2</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="C7" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="15">
         <v>3</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="15">
         <v>4</v>
       </c>
       <c r="C9" s="22"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="15">
         <v>5</v>
       </c>
       <c r="C10" s="22"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="15">
         <v>6</v>
       </c>
       <c r="C11" s="22"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="15">
         <v>7</v>
       </c>
       <c r="C12" s="22"/>
-      <c r="P12" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="15">
         <v>8</v>
       </c>
       <c r="C13" s="22"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="15">
         <v>9</v>
       </c>
       <c r="C14" s="22"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="15">
         <v>10</v>
       </c>
       <c r="C15" s="22"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="15">
         <v>11</v>
       </c>
       <c r="C16" s="22"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="15">
         <v>12</v>
       </c>
       <c r="C17" s="22"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="15">
         <v>13</v>
       </c>
       <c r="C18" s="22"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="15">
         <v>14</v>
       </c>
       <c r="C19" s="22"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="15">
         <v>15</v>
       </c>
       <c r="C20" s="22"/>
-      <c r="J20" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="K20" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="M20" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="15">
         <v>16</v>
       </c>
       <c r="C21" s="23"/>
-      <c r="I21" s="15">
-        <v>0</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="L21" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="M21" s="15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
@@ -1313,23 +1277,8 @@
       <c r="F22" s="24"/>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
-      <c r="I22" s="24">
-        <v>1</v>
-      </c>
-      <c r="J22" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="L22" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="M22" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="24"/>
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
@@ -1337,43 +1286,16 @@
       <c r="F23" s="24"/>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
-      <c r="I23" s="24">
-        <v>2</v>
-      </c>
-      <c r="J23" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="K23" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="L23" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="M23" s="15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
       <c r="E24" s="25"/>
       <c r="F24" s="25"/>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
-      <c r="I24" s="24">
-        <v>3</v>
-      </c>
-      <c r="J24" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="K24" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="L24" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="15">
         <v>0</v>
       </c>
@@ -1381,255 +1303,141 @@
         <v>7</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
-      <c r="I25" s="24">
-        <v>4</v>
-      </c>
-      <c r="J25" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="K25" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="L25" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="15">
         <v>1</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="24"/>
+        <v>32</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24" t="s">
+        <v>33</v>
+      </c>
       <c r="F26" s="24"/>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
-      <c r="I26" s="24">
-        <v>5</v>
-      </c>
-      <c r="J26" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="K26" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="L26" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="15">
         <v>2</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>35</v>
+        <v>78</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>79</v>
       </c>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
-      <c r="I27" s="24">
-        <v>6</v>
-      </c>
-      <c r="J27" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K27" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="L27" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="15">
         <v>3</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>36</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E28" s="24"/>
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
-      <c r="I28" s="24">
-        <v>7</v>
-      </c>
-      <c r="J28" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="K28" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="L28" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="15">
         <v>4</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F29" s="24"/>
       <c r="G29" s="24"/>
       <c r="H29" s="24"/>
-      <c r="I29" s="24">
-        <v>8</v>
-      </c>
-      <c r="J29" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K29" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="L29" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="24"/>
       <c r="C30" s="24"/>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
       <c r="G30" s="24"/>
       <c r="H30" s="24"/>
-      <c r="I30" s="24">
-        <v>9</v>
-      </c>
-      <c r="J30" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="K30" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="L30" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="15">
         <v>0</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
       <c r="H31" s="24"/>
-      <c r="I31" s="24">
-        <v>10</v>
-      </c>
-      <c r="J31" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="K31" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="L31" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="15">
         <v>1</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D32" s="24"/>
       <c r="F32" s="24"/>
       <c r="G32" s="24"/>
       <c r="H32" s="24"/>
-      <c r="I32" s="15">
-        <v>11</v>
-      </c>
-      <c r="J32" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="K32" s="24"/>
-      <c r="L32" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" s="15">
         <v>2</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
       <c r="H33" s="24"/>
-      <c r="K33" s="24"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="24">
         <v>22</v>
       </c>
-      <c r="C34" s="27"/>
+      <c r="C34" s="23"/>
       <c r="E34" s="24"/>
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
       <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="24"/>
       <c r="C35" s="24"/>
       <c r="E35" s="24"/>
       <c r="F35" s="24"/>
       <c r="G35" s="24"/>
       <c r="H35" s="24"/>
-      <c r="I35" s="24">
-        <v>50</v>
-      </c>
-      <c r="J35" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="K35" s="24"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="24"/>
       <c r="C36" s="24"/>
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
       <c r="G36" s="24"/>
       <c r="H36" s="24"/>
-      <c r="I36" s="24">
-        <v>51</v>
-      </c>
-      <c r="J36" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="K36" s="24"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="24"/>
       <c r="C37" s="24"/>
       <c r="E37" s="24"/>
@@ -1639,7 +1447,7 @@
       <c r="I37" s="24"/>
       <c r="J37" s="24"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B38" s="24"/>
       <c r="C38" s="24"/>
       <c r="E38" s="24"/>
@@ -1649,7 +1457,7 @@
       <c r="I38" s="24"/>
       <c r="J38" s="24"/>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B39" s="24"/>
       <c r="C39" s="24"/>
       <c r="E39" s="24"/>
@@ -1659,7 +1467,7 @@
       <c r="I39" s="24"/>
       <c r="J39" s="24"/>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" s="24"/>
       <c r="C40" s="24"/>
       <c r="E40" s="24"/>
@@ -1669,7 +1477,7 @@
       <c r="I40" s="24"/>
       <c r="J40" s="24"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B41" s="24"/>
       <c r="C41" s="24"/>
       <c r="E41" s="24"/>
@@ -1679,7 +1487,7 @@
       <c r="I41" s="24"/>
       <c r="J41" s="24"/>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42" s="24"/>
       <c r="C42" s="24"/>
       <c r="E42" s="24"/>
@@ -1689,7 +1497,7 @@
       <c r="I42" s="24"/>
       <c r="J42" s="24"/>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" s="24"/>
       <c r="C43" s="24"/>
       <c r="E43" s="24"/>
@@ -1699,7 +1507,7 @@
       <c r="I43" s="24"/>
       <c r="J43" s="24"/>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B44" s="24"/>
       <c r="C44" s="24"/>
       <c r="D44" s="24"/>
@@ -1710,7 +1518,7 @@
       <c r="I44" s="24"/>
       <c r="J44" s="24"/>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B45" s="24"/>
       <c r="C45" s="24"/>
       <c r="D45" s="24"/>
@@ -1721,7 +1529,7 @@
       <c r="I45" s="24"/>
       <c r="J45" s="24"/>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B46" s="24"/>
       <c r="C46" s="24"/>
       <c r="D46" s="24"/>
@@ -1732,7 +1540,7 @@
       <c r="I46" s="24"/>
       <c r="J46" s="24"/>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B47" s="24"/>
       <c r="C47" s="24"/>
       <c r="D47" s="24"/>
@@ -1743,7 +1551,7 @@
       <c r="I47" s="24"/>
       <c r="J47" s="24"/>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="E48" s="24"/>
       <c r="F48" s="24"/>
       <c r="G48" s="24"/>
@@ -1897,7 +1705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -2313,13 +2121,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>14</v>
-      </c>
       <c r="E4" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.15">
@@ -2327,10 +2135,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.15">
@@ -2372,10 +2180,10 @@
         <v>0</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
@@ -2387,13 +2195,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.15">
@@ -2402,7 +2210,7 @@
         <v>21</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.15">
@@ -2411,16 +2219,16 @@
         <v>358</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I14" s="1">
         <v>17</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.15">
@@ -2441,10 +2249,10 @@
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="10"/>
@@ -2478,10 +2286,10 @@
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -2506,4 +2314,276 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="15">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="24">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="24">
+        <v>2</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="24">
+        <v>3</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="24">
+        <v>4</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="24">
+        <v>5</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="24">
+        <v>6</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="24">
+        <v>7</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="24">
+        <v>8</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="24">
+        <v>9</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="24">
+        <v>10</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="15">
+        <v>11</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="24">
+        <v>50</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="24">
+        <v>51</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Minor updates to characters
</commit_message>
<xml_diff>
--- a/Docs/Rogue Packets.xlsx
+++ b/Docs/Rogue Packets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="225" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="480" yWindow="225" windowWidth="24240" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="C64 to Server" sheetId="5" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
   <si>
     <t>Byte#</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Player name in PETSCII (15 Bytes)</t>
   </si>
   <si>
-    <t>Broadcast Messages</t>
-  </si>
-  <si>
     <t>CHAT MESSAGES</t>
   </si>
   <si>
@@ -259,6 +256,21 @@
   </si>
   <si>
     <t>reserved</t>
+  </si>
+  <si>
+    <t>Screen Message #1</t>
+  </si>
+  <si>
+    <t>Screen Message #2</t>
+  </si>
+  <si>
+    <t>Screen Message #3</t>
+  </si>
+  <si>
+    <t>Screen Message #4</t>
+  </si>
+  <si>
+    <t>Screen Message #5</t>
   </si>
 </sst>
 </file>
@@ -728,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C21"/>
     </sheetView>
   </sheetViews>
@@ -1133,7 +1145,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="2:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1172,7 +1184,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
@@ -1180,7 +1192,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -1303,10 +1315,10 @@
         <v>7</v>
       </c>
       <c r="D25" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="24" t="s">
         <v>44</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>45</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="24"/>
@@ -1317,11 +1329,11 @@
         <v>1</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="24"/>
       <c r="E26" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F26" s="24"/>
       <c r="G26" s="24"/>
@@ -1332,10 +1344,10 @@
         <v>2</v>
       </c>
       <c r="C27" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>78</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>79</v>
       </c>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
@@ -1346,7 +1358,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
@@ -1358,7 +1370,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F29" s="24"/>
       <c r="G29" s="24"/>
@@ -1377,10 +1389,10 @@
         <v>0</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
@@ -1392,7 +1404,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D32" s="24"/>
       <c r="F32" s="24"/>
@@ -1404,7 +1416,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
@@ -1703,16 +1715,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="8.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
@@ -2201,7 +2213,7 @@
         <v>18</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.15">
@@ -2210,7 +2222,7 @@
         <v>21</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.15">
@@ -2219,7 +2231,7 @@
         <v>358</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>19</v>
@@ -2228,7 +2240,7 @@
         <v>17</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.15">
@@ -2236,23 +2248,40 @@
         <f>B14+40</f>
         <v>398</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B16" s="1">
+        <f>B15+40</f>
+        <v>438</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B17" s="1">
+        <f t="shared" ref="B17:B18" si="0">B16+40</f>
+        <v>478</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>23</v>
+      <c r="B18" s="1">
+        <f t="shared" ref="B18" si="1">B16+I14</f>
+        <v>455</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="10"/>
@@ -2260,37 +2289,28 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
+      <c r="B19" s="1">
+        <f>B18+40</f>
+        <v>495</v>
+      </c>
       <c r="H19" s="9"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>24</v>
-      </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -2309,6 +2329,36 @@
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B27" s="9"/>
+      <c r="C27" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B31" s="9"/>
+      <c r="C31" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2336,16 +2386,16 @@
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="15"/>
       <c r="C2" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" s="15"/>
     </row>
@@ -2354,14 +2404,14 @@
         <v>0</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" s="15"/>
     </row>
@@ -2370,16 +2420,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" s="15"/>
     </row>
@@ -2388,16 +2438,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -2406,13 +2456,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
@@ -2422,13 +2472,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
@@ -2438,13 +2488,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>39</v>
-      </c>
       <c r="E8" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
@@ -2454,13 +2504,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
@@ -2470,13 +2520,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
@@ -2486,13 +2536,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
@@ -2502,13 +2552,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
@@ -2518,13 +2568,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
@@ -2534,11 +2584,11 @@
         <v>11</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
@@ -2564,7 +2614,7 @@
         <v>50</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="15"/>
@@ -2576,7 +2626,7 @@
         <v>51</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="15"/>

</xml_diff>

<commit_message>
Messages and Health Implemented
</commit_message>
<xml_diff>
--- a/Docs/Rogue Packets.xlsx
+++ b/Docs/Rogue Packets.xlsx
@@ -270,9 +270,6 @@
     <t>Screen Message #4</t>
   </si>
   <si>
-    <t>Screen Message #5</t>
-  </si>
-  <si>
     <t>Item underneath current position</t>
   </si>
   <si>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>3 bytes</t>
+  </si>
+  <si>
+    <t>End of Packet (255)</t>
   </si>
 </sst>
 </file>
@@ -1753,7 +1753,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="8.25" x14ac:dyDescent="0.15"/>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B17" s="1">
-        <f t="shared" ref="B17:B18" si="0">B16+40</f>
+        <f t="shared" ref="B17" si="0">B16+40</f>
         <v>478</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -2315,8 +2315,11 @@
         <f>B17+40</f>
         <v>518</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="28" t="s">
         <v>84</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="10"/>
@@ -2325,14 +2328,14 @@
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="9"/>
       <c r="B19" s="1">
-        <f>B18+40</f>
-        <v>558</v>
+        <f>B18+1</f>
+        <v>519</v>
       </c>
       <c r="C19" s="28" t="s">
         <v>85</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="10"/>
@@ -2342,13 +2345,13 @@
       <c r="A20" s="9"/>
       <c r="B20" s="1">
         <f>B19+1</f>
-        <v>559</v>
+        <v>520</v>
       </c>
       <c r="C20" s="28" t="s">
         <v>86</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -2358,7 +2361,7 @@
       <c r="A21" s="9"/>
       <c r="B21" s="1">
         <f>B20+1</f>
-        <v>560</v>
+        <v>521</v>
       </c>
       <c r="C21" s="28" t="s">
         <v>87</v>
@@ -2373,13 +2376,10 @@
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="9"/>
       <c r="B22" s="1">
-        <f>B21+1</f>
-        <v>561</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="1" t="s">
+        <f>B21+3</f>
+        <v>524</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>90</v>
       </c>
       <c r="H22" s="9"/>
@@ -2387,10 +2387,6 @@
       <c r="J22" s="9"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B23" s="1">
-        <f>B22+3</f>
-        <v>564</v>
-      </c>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>

</xml_diff>

<commit_message>
Very simple SoundFX implemented
</commit_message>
<xml_diff>
--- a/Docs/Rogue Packets.xlsx
+++ b/Docs/Rogue Packets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="225" windowWidth="24240" windowHeight="13740" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="285" windowWidth="24240" windowHeight="13680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="C64 to Server" sheetId="5" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="89">
   <si>
     <t>Byte#</t>
   </si>
@@ -84,18 +84,6 @@
     <t>Player name in PETSCII (15 Bytes)</t>
   </si>
   <si>
-    <t>CHAT MESSAGES</t>
-  </si>
-  <si>
-    <t>SOUND EFFECTS</t>
-  </si>
-  <si>
-    <t>Packet Type = 130</t>
-  </si>
-  <si>
-    <t>Packet Type = 131</t>
-  </si>
-  <si>
     <t>Character type</t>
   </si>
   <si>
@@ -289,6 +277,12 @@
   </si>
   <si>
     <t>End of Packet (255)</t>
+  </si>
+  <si>
+    <t>Sound FX Counter</t>
+  </si>
+  <si>
+    <t>Sound FX ID</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1174,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="2:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1219,7 +1213,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
@@ -1227,7 +1221,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -1350,10 +1344,10 @@
         <v>7</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="24"/>
@@ -1364,11 +1358,11 @@
         <v>1</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D26" s="24"/>
       <c r="E26" s="24" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F26" s="24"/>
       <c r="G26" s="24"/>
@@ -1379,10 +1373,10 @@
         <v>2</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
@@ -1393,7 +1387,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
@@ -1405,7 +1399,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F29" s="24"/>
       <c r="G29" s="24"/>
@@ -1424,10 +1418,10 @@
         <v>0</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
@@ -1439,7 +1433,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D32" s="24"/>
       <c r="F32" s="24"/>
@@ -1451,7 +1445,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
@@ -1750,10 +1744,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="8.25" x14ac:dyDescent="0.15"/>
@@ -2248,7 +2242,7 @@
         <v>18</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.15">
@@ -2257,7 +2251,7 @@
         <v>21</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.15">
@@ -2266,7 +2260,7 @@
         <v>358</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>19</v>
@@ -2275,7 +2269,7 @@
         <v>17</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.15">
@@ -2284,7 +2278,7 @@
         <v>398</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.15">
@@ -2293,7 +2287,7 @@
         <v>438</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J16" s="8"/>
     </row>
@@ -2303,7 +2297,7 @@
         <v>478</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -2316,10 +2310,10 @@
         <v>518</v>
       </c>
       <c r="C18" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="10"/>
@@ -2332,10 +2326,10 @@
         <v>519</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="10"/>
@@ -2348,10 +2342,10 @@
         <v>520</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -2364,10 +2358,10 @@
         <v>521</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -2379,19 +2373,42 @@
         <f>B21+3</f>
         <v>524</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>90</v>
+      <c r="C22" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B23" s="1">
+        <f>B22+1</f>
+        <v>525</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B24" s="1">
+        <f>B23+1</f>
+        <v>526</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -2401,35 +2418,50 @@
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B27" s="9"/>
-      <c r="C27" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B31" s="9"/>
-      <c r="C31" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>23</v>
-      </c>
+    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+    </row>
+    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+    </row>
+    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2457,16 +2489,16 @@
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="15"/>
       <c r="C2" s="16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G2" s="15"/>
     </row>
@@ -2475,14 +2507,14 @@
         <v>0</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G3" s="15"/>
     </row>
@@ -2491,16 +2523,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G4" s="15"/>
     </row>
@@ -2509,16 +2541,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -2527,13 +2559,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
@@ -2543,13 +2575,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
@@ -2559,13 +2591,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
@@ -2575,13 +2607,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
@@ -2591,13 +2623,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
@@ -2607,13 +2639,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
@@ -2623,13 +2655,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
@@ -2639,13 +2671,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
@@ -2655,11 +2687,11 @@
         <v>11</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
@@ -2685,7 +2717,7 @@
         <v>50</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="15"/>
@@ -2697,7 +2729,7 @@
         <v>51</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="15"/>

</xml_diff>